<commit_message>
- added room details page - room list page
</commit_message>
<xml_diff>
--- a/SRS.xlsx
+++ b/SRS.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data fields" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>date</t>
   </si>
@@ -263,6 +263,33 @@
   </si>
   <si>
     <t>refering to user</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Found on</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Page / application Url</t>
+  </si>
+  <si>
+    <t>/newRoom_details</t>
+  </si>
+  <si>
+    <t>the validation for the price and the capacity shows error for single digit</t>
   </si>
 </sst>
 </file>
@@ -333,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,6 +381,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
@@ -1139,13 +1169,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30">
+      <c r="A2" s="8">
+        <v>42609</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="8">
+        <v>42609</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
- added filter for the room type for get rooms
</commit_message>
<xml_diff>
--- a/SRS.xlsx
+++ b/SRS.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data fields" sheetId="1" r:id="rId1"/>
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Enhancements" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="99">
   <si>
     <t>date</t>
   </si>
@@ -290,6 +290,42 @@
   </si>
   <si>
     <t>the validation for the price and the capacity shows error for single digit</t>
+  </si>
+  <si>
+    <t>/room(GET)</t>
+  </si>
+  <si>
+    <t>rajashree</t>
+  </si>
+  <si>
+    <t>19-9-16</t>
+  </si>
+  <si>
+    <t>add extra parameter for the filter as roomType in the client side</t>
+  </si>
+  <si>
+    <t>add extra parameter for the filter as roomType in the server side</t>
+  </si>
+  <si>
+    <t>rajendra</t>
+  </si>
+  <si>
+    <t>/room(POST)</t>
+  </si>
+  <si>
+    <t>while saving room make the room type as mandaroty to select any one , in client side</t>
+  </si>
+  <si>
+    <t>while saving room make the room type as mandaroty to select any one , in server side</t>
+  </si>
+  <si>
+    <t>In the client side show the validation error so that the user could know where the validation is not proper</t>
+  </si>
+  <si>
+    <t>This can be done using the alert of the ui bootstrap</t>
+  </si>
+  <si>
+    <t>Error not proper for the auth in the server console</t>
   </si>
 </sst>
 </file>
@@ -1171,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1236,12 +1272,234 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30">
+      <c r="A2" s="8">
+        <v>42632</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
+      <c r="A3" s="8">
+        <v>42632</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="8">
+        <v>42633</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="8">
+        <v>42634</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45">
+      <c r="A6" s="8">
+        <v>42635</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45">
+      <c r="A7" s="8">
+        <v>42636</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8">
+        <v>42637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8">
+        <v>42638</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="8">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8">
+        <v>42641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8">
+        <v>42642</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="8">
+        <v>42643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="8">
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="8">
+        <v>42645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="8">
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="8">
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="8">
+        <v>42648</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="8">
+        <v>42649</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- update room filter -fixed some validation issues in the server side
</commit_message>
<xml_diff>
--- a/SRS.xlsx
+++ b/SRS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
   <si>
     <t>date</t>
   </si>
@@ -326,13 +326,56 @@
   </si>
   <si>
     <t>Error not proper for the auth in the server console</t>
+  </si>
+  <si>
+    <t>Done , for more check the api docs</t>
+  </si>
+  <si>
+    <t>/room(PUT)</t>
+  </si>
+  <si>
+    <t>while updating room the invalid data for the room type do not show error but also not adding the errorneous data like if add any room type except the enum values then not show error on update</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">This is due to mongoose do not validate in case of update
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for that we need to validation in controller before update in the mongoose
+orelse we can find the record then .save() so that the validation in model layer will work</t>
+    </r>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>server side in case of the dash board the rooms must be consider that are not deleted</t>
+  </si>
+  <si>
+    <t>Done , need to add one condition in $match</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +402,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -396,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +469,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1272,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1288,7 +1343,8 @@
     <col min="6" max="6" width="21.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
@@ -1317,35 +1373,35 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
-      <c r="A2" s="8">
+    <row r="2" spans="1:8" s="10" customFormat="1" ht="30">
+      <c r="A2" s="9">
         <v>42632</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30">
-      <c r="A3" s="8">
+      <c r="E2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="45">
+      <c r="A3" s="9">
         <v>42632</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>91</v>
+      <c r="C3" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>92</v>
@@ -1356,150 +1412,207 @@
       <c r="F3" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="G3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="8">
-        <v>42633</v>
+        <v>42632</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>89</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>89</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
       <c r="A5" s="8">
-        <v>42634</v>
+        <v>42633</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="8">
+        <v>42634</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="8">
-        <v>42635</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="E6" s="8" t="s">
         <v>89</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="G6" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45">
       <c r="A7" s="8">
+        <v>42635</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45">
+      <c r="A8" s="8">
         <v>42636</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="8">
+      <c r="E8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="195">
+      <c r="A9" s="8">
         <v>42637</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="8">
-        <v>42638</v>
+      <c r="B9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="8">
-        <v>42639</v>
+        <v>42638</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="8">
-        <v>42640</v>
+        <v>42639</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="8">
-        <v>42641</v>
+        <v>42640</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="8">
-        <v>42642</v>
+        <v>42641</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="8">
-        <v>42643</v>
+        <v>42642</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="8">
-        <v>42644</v>
+        <v>42643</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="8">
-        <v>42645</v>
+        <v>42644</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="8">
-        <v>42646</v>
+        <v>42645</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="8">
-        <v>42647</v>
+        <v>42646</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="8">
-        <v>42648</v>
+        <v>42647</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="8">
+        <v>42648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="8">
         <v>42649</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- added web service for the reports
</commit_message>
<xml_diff>
--- a/SRS.xlsx
+++ b/SRS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
   <si>
     <t>date</t>
   </si>
@@ -369,6 +369,24 @@
   </si>
   <si>
     <t>Done , need to add one condition in $match</t>
+  </si>
+  <si>
+    <t>/reports(get)</t>
+  </si>
+  <si>
+    <t>server side change to get the reports on the basis of start date and the end date from the reports table</t>
+  </si>
+  <si>
+    <t>Now it is fetching from the trasaction table for now need to be change</t>
+  </si>
+  <si>
+    <t>spelling mistake</t>
+  </si>
+  <si>
+    <t>the model mapping of transaction model mistake as tranctionModelObj</t>
+  </si>
+  <si>
+    <t>need to change in all the resp controller and files</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1551,14 +1569,50 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="8">
         <v>42638</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="B10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="8">
         <v>42639</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8">

</xml_diff>